<commit_message>
Today Defect Task Completed and Updated
</commit_message>
<xml_diff>
--- a/samhitha_automation_scripts/samhitha_data/Samhithasoft_Saranya.xlsx
+++ b/samhitha_automation_scripts/samhitha_data/Samhithasoft_Saranya.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\SamhithaSoftware\samhithasoftware_testing\samhitha_software_automation_Scripts\samhitha_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Samhitha_Project_Version2\samhitha_version2\samhitha_automation_scripts\samhitha_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3743" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3743" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="HP_Scenarios" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Our_Achievements_Testcase" sheetId="11" r:id="rId11"/>
     <sheet name="Our_Achievements_TracebilityMa" sheetId="12" r:id="rId12"/>
     <sheet name="Our_Achievements_Defect" sheetId="13" r:id="rId13"/>
+    <sheet name="Defect_27_3_Task" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="841">
   <si>
     <t>SS_HP_S1</t>
   </si>
@@ -2300,12 +2301,297 @@
   <si>
     <t>When user click on "Play" button in Our Achievement page, it should play video on same page</t>
   </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>S.No:</t>
+  </si>
+  <si>
+    <t>About Us Page</t>
+  </si>
+  <si>
+    <t>Font should be changed in new font</t>
+  </si>
+  <si>
+    <t>Displaying old font</t>
+  </si>
+  <si>
+    <t>Samhitha Software should be display</t>
+  </si>
+  <si>
+    <t>Displaying Samhitha soft,in the bottom of the About Us page instead of Samhitha Software</t>
+  </si>
+  <si>
+    <t>Our Achievements</t>
+  </si>
+  <si>
+    <t>What We Are</t>
+  </si>
+  <si>
+    <t>Samhitha Software should be display everywhere</t>
+  </si>
+  <si>
+    <t>Displaying Samhitha soft,in the bottom of the Our Achievement page instead of Samhitha Software</t>
+  </si>
+  <si>
+    <t>Samhihta Software is displaying in the top of the What We Are page insteaded of Samhitha Software(spel mis)</t>
+  </si>
+  <si>
+    <t>Displaying Samhitha soft,in the bottom of the What We Are page instead of Samhitha Software</t>
+  </si>
+  <si>
+    <t>Company Profile</t>
+  </si>
+  <si>
+    <t>Ring Slider is not there</t>
+  </si>
+  <si>
+    <t>What We Do</t>
+  </si>
+  <si>
+    <t>Email id should be changed to info@samhitha software.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In middle of What We Do page ,Email id is not be changed, is displaying padmini@samhithasoftware.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In middle of What We Do page ,Phone number is not be changed, is displaying +91 8049798777</t>
+  </si>
+  <si>
+    <t>Spell mistaken in address(Mahadevapura)</t>
+  </si>
+  <si>
+    <t>Mahadevpura and Mahadepura is displaying in the middle of What We Do page</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Management Team</t>
+  </si>
+  <si>
+    <t>Opened with same tab</t>
+  </si>
+  <si>
+    <t>When click on Management TeamTab, Management Team page it should open with new tab</t>
+  </si>
+  <si>
+    <t>In Sundeep Information ,in the third line Samhitha only displaying instead Samhitha Software</t>
+  </si>
+  <si>
+    <t>In Nameshwara Rao Information ,in the first line Samhitha only displaying instead Samhitha Software</t>
+  </si>
+  <si>
+    <t>Dulicate date</t>
+  </si>
+  <si>
+    <t>In Ashish Mishra Information, Nameshwara rao informarions are displaying</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Awards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programs </t>
+  </si>
+  <si>
+    <t>Programs Page is not working</t>
+  </si>
+  <si>
+    <t>Seminars And Workshops</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence &amp; Deep Learning</t>
+  </si>
+  <si>
+    <t>Font Mistake</t>
+  </si>
+  <si>
+    <t>In Services tab ,first letter in small (services)</t>
+  </si>
+  <si>
+    <t>All the 3 ring sliders having same informations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ring Slider info </t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate Page </t>
+  </si>
+  <si>
+    <t>UI UX Designes</t>
+  </si>
+  <si>
+    <t>Duplicate Page</t>
+  </si>
+  <si>
+    <t>Data Science Programs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industries </t>
+  </si>
+  <si>
+    <t>Page is not working</t>
+  </si>
+  <si>
+    <t>Title Font Mistake(Ecommerce)</t>
+  </si>
+  <si>
+    <t>Ecommerce is displaying instead of E-commerce</t>
+  </si>
+  <si>
+    <t>E-commerce</t>
+  </si>
+  <si>
+    <t>when user clicks on E-commerce tab , it should open in new tab</t>
+  </si>
+  <si>
+    <t>E-commerce page is open in same tab</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Media &amp; Entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthcare &amp; Lifescience </t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>when user clicks on Logistics tab , it should open in new tab</t>
+  </si>
+  <si>
+    <t>Logistics page is open in same tab</t>
+  </si>
+  <si>
+    <t>Title Mistake , no special char should added in the title</t>
+  </si>
+  <si>
+    <t>In Cargo Management Solutions Tab, (Cargo Management Solutions:) is displaying instead of Cargo Management Solutions</t>
+  </si>
+  <si>
+    <t>Energy and Utilities</t>
+  </si>
+  <si>
+    <t>Food And Beverages</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Air Lines</t>
+  </si>
+  <si>
+    <t>Travels and Hospitality</t>
+  </si>
+  <si>
+    <t>Banking &amp; Finance</t>
+  </si>
+  <si>
+    <t>Telecom</t>
+  </si>
+  <si>
+    <t>Purple Glossy</t>
+  </si>
+  <si>
+    <t>Hi Skill</t>
+  </si>
+  <si>
+    <t>Lease IT</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Capabilities</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>IT Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In IT Service Management (ITSM) Tab,IT Service Management (ITSM) : is displaying instead of IT Service Management (ITSM) </t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Services Details</t>
+  </si>
+  <si>
+    <t>Title not matched (url title not matched)</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>Minor Tab not displaying proparely (hiding)</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>Displaying Samhitha soft,in the bottom of the page instead of Samhitha Software</t>
+  </si>
+  <si>
+    <t>Phone number in bottom of page not be changed to +91 9845937999, is displaying +91 8049798777</t>
+  </si>
+  <si>
+    <t>In all pages phone number should be changed to +91 9845937999</t>
+  </si>
+  <si>
+    <t>In all pages Email id should be changed to info@samhithasoftware.com</t>
+  </si>
+  <si>
+    <t>Find Duplicate Page</t>
+  </si>
+  <si>
+    <t>Check Old fonts should changed into New Font</t>
+  </si>
+  <si>
+    <t>Everwhere Samhitha Software should be displayed (Instead of Samhitha )</t>
+  </si>
+  <si>
+    <t>Phone Number should be changed to +91 9845937999</t>
+  </si>
+  <si>
+    <t>Phone Number in bottom of Our Achievement page not be changed to +91 9845937999, is displaying +91 8049798777</t>
+  </si>
+  <si>
+    <t>Phone Number in bottom of About Us page not be changed to +91 9845937999, is displaying +91 8049798777</t>
+  </si>
+  <si>
+    <t>Phone Number in bottom of the page not be changed to +91 9845937999, is displaying +91 8049798777</t>
+  </si>
+  <si>
+    <t>Phone Number in bottom of page not be changed to +91 9845937999, is displaying +91 8049798777</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Displaying Samhitha soft,in the bottom of the page instead of Samhitha Software,in Address Area</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2364,6 +2650,24 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2553,7 +2857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2672,6 +2976,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3087,7 +3394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A112" workbookViewId="0">
       <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
@@ -3984,7 +4291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
+    <sheetView topLeftCell="A170" workbookViewId="0">
       <selection activeCell="A199" sqref="A199"/>
     </sheetView>
   </sheetViews>
@@ -5894,6 +6201,2153 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E199"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.06640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.53125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A1" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="66">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="66">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="66">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="66">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="66">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="66"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A8" s="65" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="66">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="65"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="66"/>
+    </row>
+    <row r="13" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>752</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>756</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A26" s="3" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="4">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="4">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>758</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="4">
+        <v>4</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="4">
+        <v>3</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="4">
+        <v>4</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A42" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
+        <v>1</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <v>2</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
+        <v>3</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <v>4</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <v>5</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>762</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
+        <v>6</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A50" s="3" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A51" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="4">
+        <v>1</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="4">
+        <v>2</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A55" s="3" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A56" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="4">
+        <v>1</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="4">
+        <v>2</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="4">
+        <v>3</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="4">
+        <v>4</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="4">
+        <v>5</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="3" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="4">
+        <v>1</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="4">
+        <v>2</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="4">
+        <v>3</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="3" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="4">
+        <v>1</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="4">
+        <v>2</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="4">
+        <v>3</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="B75" s="64" t="s">
+        <v>778</v>
+      </c>
+      <c r="C75" s="64"/>
+      <c r="D75" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D76" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="3" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="4">
+        <v>1</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="4">
+        <v>2</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="4">
+        <v>3</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A83" s="3" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="4">
+        <v>1</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="4">
+        <v>2</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="4">
+        <v>3</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="4">
+        <v>4</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="4">
+        <v>5</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="64" t="s">
+        <v>785</v>
+      </c>
+      <c r="B91" s="64" t="s">
+        <v>786</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="64"/>
+      <c r="B92" s="64"/>
+      <c r="D92" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="64"/>
+      <c r="B93" s="64"/>
+    </row>
+    <row r="95" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="64" t="s">
+        <v>787</v>
+      </c>
+      <c r="B95" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A96" s="64"/>
+      <c r="B96" s="64"/>
+      <c r="D96" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="64"/>
+      <c r="B97" s="64"/>
+    </row>
+    <row r="99" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="64" t="s">
+        <v>789</v>
+      </c>
+      <c r="B99" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A100" s="64"/>
+      <c r="B100" s="64"/>
+      <c r="D100" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A101" s="64"/>
+      <c r="B101" s="64"/>
+    </row>
+    <row r="103" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="64" t="s">
+        <v>790</v>
+      </c>
+      <c r="B103" s="64" t="s">
+        <v>791</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="64"/>
+      <c r="B104" s="64"/>
+      <c r="D104" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A105" s="64"/>
+      <c r="B105" s="64"/>
+    </row>
+    <row r="106" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A106" s="64"/>
+      <c r="B106" s="64"/>
+    </row>
+    <row r="108" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="3" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A109" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="4">
+        <v>1</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" s="4">
+        <v>2</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="4">
+        <v>3</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" s="4">
+        <v>4</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="64" t="s">
+        <v>797</v>
+      </c>
+      <c r="B115" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A116" s="64"/>
+      <c r="B116" s="64"/>
+      <c r="D116" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A118" s="64" t="s">
+        <v>798</v>
+      </c>
+      <c r="B118" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A119" s="64"/>
+      <c r="B119" s="64"/>
+      <c r="D119" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A121" s="64" t="s">
+        <v>799</v>
+      </c>
+      <c r="B121" s="64" t="s">
+        <v>800</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A122" s="64"/>
+      <c r="B122" s="64"/>
+      <c r="D122" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A124" s="3" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A125" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" s="4">
+        <v>1</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>803</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" s="4">
+        <v>2</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" s="4">
+        <v>3</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" s="4">
+        <v>4</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A131" s="64" t="s">
+        <v>806</v>
+      </c>
+      <c r="B131" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A132" s="64"/>
+      <c r="B132" s="64"/>
+      <c r="D132" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A134" s="3" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A135" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" s="4">
+        <v>1</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" s="4">
+        <v>2</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A139" s="64" t="s">
+        <v>808</v>
+      </c>
+      <c r="B139" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A140" s="64"/>
+      <c r="B140" s="64"/>
+      <c r="D140" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A142" s="64" t="s">
+        <v>809</v>
+      </c>
+      <c r="B142" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A143" s="64"/>
+      <c r="B143" s="64"/>
+      <c r="D143" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A144" s="64"/>
+    </row>
+    <row r="145" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A145" s="64" t="s">
+        <v>810</v>
+      </c>
+      <c r="B145" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A146" s="64"/>
+      <c r="B146" s="64"/>
+      <c r="D146" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A147" s="64"/>
+    </row>
+    <row r="148" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A148" s="64" t="s">
+        <v>811</v>
+      </c>
+      <c r="B148" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A149" s="64"/>
+      <c r="B149" s="64"/>
+      <c r="D149" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A150" s="64"/>
+    </row>
+    <row r="151" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A151" s="64" t="s">
+        <v>812</v>
+      </c>
+      <c r="B151" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A152" s="64"/>
+      <c r="B152" s="64"/>
+      <c r="D152" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A153" s="64"/>
+    </row>
+    <row r="154" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A154" s="64" t="s">
+        <v>813</v>
+      </c>
+      <c r="B154" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A155" s="64"/>
+      <c r="B155" s="64"/>
+      <c r="D155" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A156" s="64"/>
+    </row>
+    <row r="157" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A157" s="64" t="s">
+        <v>814</v>
+      </c>
+      <c r="B157" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A158" s="64"/>
+      <c r="B158" s="64"/>
+      <c r="D158" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A159" s="64"/>
+    </row>
+    <row r="160" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A160" s="64" t="s">
+        <v>815</v>
+      </c>
+      <c r="B160" s="64" t="s">
+        <v>788</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A161" s="64"/>
+      <c r="B161" s="64"/>
+      <c r="D161" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A162" s="64"/>
+      <c r="B162" s="64"/>
+    </row>
+    <row r="164" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A164" s="3" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A165" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="4">
+        <v>1</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" s="4">
+        <v>2</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" s="4">
+        <v>3</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E168" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A170" s="3" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A171" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" s="4">
+        <v>1</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" s="4">
+        <v>2</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" s="4">
+        <v>3</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A176" s="3" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A177" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178" s="4">
+        <v>1</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E178" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179" s="4">
+        <v>2</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E179" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180" s="4">
+        <v>3</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E180" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A182" s="3" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A183" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184" s="4">
+        <v>1</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E184" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185" s="4">
+        <v>2</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E185" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A187" s="3" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A188" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189" s="4">
+        <v>1</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E189" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A190" s="4">
+        <v>2</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E190" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191" s="4">
+        <v>3</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E191" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A193" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A195" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A197" s="3" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A198" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" s="4">
+        <v>1</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E199" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10430,12 +12884,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B10:D10"/>
@@ -10443,6 +12891,12 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Our achivement page tc updated
</commit_message>
<xml_diff>
--- a/samhitha_automation_scripts/samhitha_data/Samhithasoft_Saranya.xlsx
+++ b/samhitha_automation_scripts/samhitha_data/Samhithasoft_Saranya.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4280" uniqueCount="1130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4352" uniqueCount="1203">
   <si>
     <t>SS_HP_S1</t>
   </si>
@@ -3453,6 +3453,225 @@
   </si>
   <si>
     <t>Mouse Hover on "Services" Tab</t>
+  </si>
+  <si>
+    <t>When user click on "Know More" button in above ring sliders in Our Achievement page, "Know More" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Know More" button in bottom of "Our Achievement" title in Our Achievement page, "Know More" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Innovative Sofware Solutions" tab in Our Achievement page,  "Innovative Sofware Solutions" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Learn More" button in the Innovative Software Solution title in Our Achievement page,  "Learn More" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Digital Marketing Mastery" tab in Our Achievement page,  "Digital Marketing Mastery" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Learn More" button in the Digital Marketing Mastery title in Our Achievement page,  "Learn More" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Global Outsourcing Execellence" tab in Our Achievement page,  "Global Outsourcing Execellence" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Learn More" button in the Global Outsourcing Execellence title in Our Achievement page,  "Learn More" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Client Satisfication Milestone" tab in Our Achievement page,  "Client Satisfication Milestone" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "Learn More" button in the Client Satisfication Milestone title in Our Achievement page,  "Learn More" page should be displayed on same page</t>
+  </si>
+  <si>
+    <t>When user click on "IT Consultant" tab in the bottam of the Our Achievement page, "IT Consultant" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Testimonials" tab in the bottam of the Our Achievement page, "Testimonials" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "IT Solutions" tab in the bottam of the Our Achievement page, "IT Solutions" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Contact Us" tab in the bottam of the Our Achievement page, "Contact Us" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Team" tab in the bottam of the Our Achievement page, "Team" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Pricing" tab in the bottam of the Our Achievement page, "Pricing" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Customers" tab in the bottam of the Our Achievement page, "Customers" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Learning Center" tab in the bottam of the Our Achievement page, "Learning Center" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Help desk" tab in the bottam of the Our Achievement page, "Learning Center" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "News" tab in the bottam of the Our Achievement page, "News" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Support" tab in the bottam of the Our Achievement page, "Support" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user hovers or takes the mouse pointer on "Facebook" link in the bottom of the Our Achievements page background of "Facebook" link/tab should get highted with violet color</t>
+  </si>
+  <si>
+    <t>When user hovers or takes the mouse pointer on"Twitter" link in the bottom of the Our Achievements page background of "Twitter" link/tab should get highted with violet  color</t>
+  </si>
+  <si>
+    <t>When user hovers or takes the mouse pointer on "Linkedin" link in the bottam of the Our Achievements page background of "Linkedin" link/tab should get highted with violet color</t>
+  </si>
+  <si>
+    <t>When user hovers or takes the mouse pointer on "Instagram" link in the bottom of the Our Achievements page background of "Instagram" link/tab should get highted with violet color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user hovers or takes the mouse pointer on "Twitter" link in the bottam of the Our Achievements page mouse cursor should get changed to hand pointer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user hovers or takes the mouse pointer on "Facebook" link in the bottam of the Our Achievements page mouse cursor should get changed to hand pointer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user hovers or takes the mouse pointer on "Linkedin"  link in the bottam of the Our Achievements page mouse cursor should get changed to hand pointer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user hovers or takes the mouse pointer on "Instagram" link in the bottam of the Our Achievements page mouse cursor should get changed to hand pointer </t>
+  </si>
+  <si>
+    <t>When user click on "Facebook" tab/link in the bottam of the Our Achievement page, "Facebook" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Twitter" tab/link in the bottam of the Our Achievement page, "Twitter" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Instagram" tab/link in the bottam of the Our Achievement page, "Instagram" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>When user click on "Linkedin" tab/link in the bottam of the Our Achievement page, "Linkedin" page should be displayed on new tab</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_110</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_111</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_112</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_113</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_114</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_115</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_116</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_117</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_118</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_119</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_120</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_121</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_122</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_123</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_124</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_125</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_126</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_127</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_128</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_129</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_130</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_131</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_132</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_133</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_134</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_135</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_136</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_137</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_138</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_139</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user enter the alphabets into "Name" text field in the Our Achievement Page, it should be accept </t>
+  </si>
+  <si>
+    <t>When user enter the special characters into  "Name" text field in the Our Achievement Page, it should show the error message</t>
+  </si>
+  <si>
+    <t>When user enter the numbers into  "Name" text field in the Our Achievement Page, it should show the error message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the user enters proper mail id into "Your Email" text field in the Our Achievement Page, it should accept </t>
+  </si>
+  <si>
+    <t>When the user enters improper mail id into "Your Email" text field in the Our Achievement Page, it should not accept</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_141</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_142</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_143</t>
+  </si>
+  <si>
+    <t>SS_OAP_SC_144</t>
   </si>
 </sst>
 </file>
@@ -4270,10 +4489,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B133"/>
+  <dimension ref="A1:B168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -5133,7 +5352,7 @@
         <v>738</v>
       </c>
       <c r="B129" s="61" t="s">
-        <v>743</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -5148,15 +5367,301 @@
       <c r="A131" s="61" t="s">
         <v>740</v>
       </c>
+      <c r="B131" s="61" t="s">
+        <v>1131</v>
+      </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="61" t="s">
         <v>741</v>
       </c>
+      <c r="B132" s="61" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="61" t="s">
         <v>742</v>
+      </c>
+      <c r="B133" s="61" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="61" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B134" s="61" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="61" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B135" s="61" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="61" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B136" s="61" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="61" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B137" s="61" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="61" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B138" s="61" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="61" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B139" s="61" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="61" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B140" s="61" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="61" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B141" s="61" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="61" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B142" s="61" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="61" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B143" s="61" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="61" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B144" s="61" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="61" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B145" s="61" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="61" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B146" s="61" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="61" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B147" s="61" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="61" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B148" s="61" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="61" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B149" s="61" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="61" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B150" s="61" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="61" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B151" s="61" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="61" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B152" s="61" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="61" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B153" s="61" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="61" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B154" s="61" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="61" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B155" s="61" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="61" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B156" s="61" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="61" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B157" s="61" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="61" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B158" s="61" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="61" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B159" s="61" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="61" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B160" s="61" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="61" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B161" s="61" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="61" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B162" s="61" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="61" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="61" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="61" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="61" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" s="61" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="61" t="s">
+        <v>1202</v>
       </c>
     </row>
   </sheetData>
@@ -18768,7 +19273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A164" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -25281,6 +25786,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B15:H15"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B10:D10"/>
@@ -25288,12 +25799,6 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25543,7 +26048,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>